<commit_message>
Feat: finished generating Implied Volatility charts
</commit_message>
<xml_diff>
--- a/data/simulation_results.xlsx
+++ b/data/simulation_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hoanghieu/projects/garch-option-pricing-seminar/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34D28C05-135A-4B4C-ABEA-C3B8BB509AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2182563A-F43E-8E40-B107-9D39A40AD930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8980" yWindow="1900" windowWidth="28200" windowHeight="20540" activeTab="1" xr2:uid="{9E06057C-7522-844E-9C65-8FDE5D1F40C0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{9E06057C-7522-844E-9C65-8FDE5D1F40C0}"/>
   </bookViews>
   <sheets>
     <sheet name="DAX" sheetId="8" r:id="rId1"/>
@@ -45,28 +45,28 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{AA8BA35D-FB59-A047-8E0F-AC63EAABE2B8}" name="result1" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/hoanghieu/projects/garch-option-pricing-seminar/data/result.csv">
+    <textPr sourceFile="/Users/hoanghieu/projects/garch-option-pricing-seminar/data/result.csv">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{6904B522-7F05-BF4E-A03D-4241D6E0A94D}" name="result111" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/hoanghieu/projects/garch-option-pricing-seminar/data/result.csv">
+    <textPr sourceFile="/Users/hoanghieu/projects/garch-option-pricing-seminar/data/result.csv">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
   <connection id="3" xr16:uid="{8FE34B07-A90E-4948-A30D-BB93CA1E4B2B}" name="result1111" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/hoanghieu/projects/garch-option-pricing-seminar/data/result.csv">
+    <textPr sourceFile="/Users/hoanghieu/projects/garch-option-pricing-seminar/data/result.csv">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
   <connection id="4" xr16:uid="{E1A04D74-D10A-BC4F-A446-DBF4FB17511B}" name="result12" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/hoanghieu/projects/garch-option-pricing-seminar/data/result.csv">
+    <textPr sourceFile="/Users/hoanghieu/projects/garch-option-pricing-seminar/data/result.csv">
       <textFields>
         <textField/>
       </textFields>
@@ -146,9 +146,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="169" formatCode="0.000000"/>
-    <numFmt numFmtId="171" formatCode="0.0000"/>
-    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -329,32 +329,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,19 +373,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_3" connectionId="3" xr16:uid="{F5B9D6A7-FD5B-2F41-92F8-84EA1E35CC54}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_1" connectionId="4" xr16:uid="{B98DA41E-5B60-EC46-89F5-B14653858411}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_3" connectionId="3" xr16:uid="{F5B9D6A7-FD5B-2F41-92F8-84EA1E35CC54}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_3" connectionId="2" xr16:uid="{2BF46B75-D266-2D45-914C-5C3DBE8E050A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_1" connectionId="1" xr16:uid="{BC2AA403-4718-2A40-9CE6-1DF59C1802B4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_1" connectionId="1" xr16:uid="{BC2AA403-4718-2A40-9CE6-1DF59C1802B4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_3" connectionId="2" xr16:uid="{2BF46B75-D266-2D45-914C-5C3DBE8E050A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -688,7 +688,7 @@
   <dimension ref="B1:O59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -779,7 +779,7 @@
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="24">
         <v>43171</v>
       </c>
     </row>
@@ -787,7 +787,7 @@
       <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="24">
         <v>44175</v>
       </c>
     </row>
@@ -798,23 +798,23 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="12">
+      <c r="E10" s="25">
         <v>0.8</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="12">
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="25">
         <v>1</v>
       </c>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="12">
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="25">
         <v>1.2</v>
       </c>
-      <c r="N10" s="12"/>
-      <c r="O10" s="14"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="26"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
@@ -846,7 +846,7 @@
       <c r="N11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="O11" s="15" t="s">
+      <c r="O11" s="13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -870,45 +870,45 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
-      <c r="O12" s="15"/>
+      <c r="O12" s="13"/>
     </row>
     <row r="13" spans="2:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="22">
+      <c r="B13" s="20">
         <v>30</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="21">
         <v>0.8</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="22">
         <v>1.44663045968903E-2</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="22">
         <v>1.38728176003902E-2</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="22">
         <v>-4.1025473542681601</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="22">
         <v>19.122679823786299</v>
       </c>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24">
+      <c r="H13" s="22"/>
+      <c r="I13" s="22">
         <v>1.5144904421229E-2</v>
       </c>
-      <c r="J13" s="24">
+      <c r="J13" s="22">
         <v>4.6908995990901996</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K13" s="22">
         <v>19.168513978454399</v>
       </c>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24">
+      <c r="L13" s="22"/>
+      <c r="M13" s="22">
         <v>1.7764570734038299E-2</v>
       </c>
-      <c r="N13" s="24">
+      <c r="N13" s="22">
         <v>22.799645307185099</v>
       </c>
-      <c r="O13" s="25">
+      <c r="O13" s="23">
         <v>23.381518102306099</v>
       </c>
     </row>
@@ -948,7 +948,7 @@
       <c r="N14" s="8">
         <v>3.0062807208140501</v>
       </c>
-      <c r="O14" s="16">
+      <c r="O14" s="14">
         <v>3.9794933232965799</v>
       </c>
     </row>
@@ -988,7 +988,7 @@
       <c r="N15" s="8">
         <v>0.80093316370797796</v>
       </c>
-      <c r="O15" s="16">
+      <c r="O15" s="14">
         <v>2.3165906118976598</v>
       </c>
     </row>
@@ -1028,7 +1028,7 @@
       <c r="N16" s="8">
         <v>0.41498589936396302</v>
       </c>
-      <c r="O16" s="16">
+      <c r="O16" s="14">
         <v>1.5094476890389501</v>
       </c>
     </row>
@@ -1068,7 +1068,7 @@
       <c r="N17" s="8">
         <v>0.92984032760688196</v>
       </c>
-      <c r="O17" s="16">
+      <c r="O17" s="14">
         <v>1.0693661618622099</v>
       </c>
     </row>
@@ -1108,7 +1108,7 @@
       <c r="N18" s="8">
         <v>-4.0792473153761E-2</v>
       </c>
-      <c r="O18" s="16">
+      <c r="O18" s="14">
         <v>0.79959783189042899</v>
       </c>
     </row>
@@ -1148,47 +1148,47 @@
       <c r="N19" s="8">
         <v>8.3525428395948096E-3</v>
       </c>
-      <c r="O19" s="16">
+      <c r="O19" s="14">
         <v>0.514655604411693</v>
       </c>
     </row>
     <row r="20" spans="2:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="22">
+      <c r="B20" s="20">
         <v>90</v>
       </c>
-      <c r="C20" s="23">
+      <c r="C20" s="21">
         <v>0.8</v>
       </c>
-      <c r="D20" s="24">
+      <c r="D20" s="22">
         <v>0.48730192285656398</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="22">
         <v>0.47701564403257901</v>
       </c>
-      <c r="F20" s="24">
+      <c r="F20" s="22">
         <v>-2.1108635820036001</v>
       </c>
-      <c r="G20" s="24">
+      <c r="G20" s="22">
         <v>4.9312084202921103</v>
       </c>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24">
+      <c r="H20" s="22"/>
+      <c r="I20" s="22">
         <v>0.48066026600690798</v>
       </c>
-      <c r="J20" s="24">
+      <c r="J20" s="22">
         <v>-1.3629449296487799</v>
       </c>
-      <c r="K20" s="24">
+      <c r="K20" s="22">
         <v>5.0823162616896997</v>
       </c>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24">
+      <c r="L20" s="22"/>
+      <c r="M20" s="22">
         <v>0.49304695397912701</v>
       </c>
-      <c r="N20" s="24">
+      <c r="N20" s="22">
         <v>1.17894694297244</v>
       </c>
-      <c r="O20" s="25">
+      <c r="O20" s="23">
         <v>5.2155040829387396</v>
       </c>
     </row>
@@ -1228,7 +1228,7 @@
       <c r="N21" s="8">
         <v>2.98016870088742</v>
       </c>
-      <c r="O21" s="16">
+      <c r="O21" s="14">
         <v>2.5626160288231299</v>
       </c>
     </row>
@@ -1268,7 +1268,7 @@
       <c r="N22" s="8">
         <v>-0.15280019798795599</v>
       </c>
-      <c r="O22" s="16">
+      <c r="O22" s="14">
         <v>1.9195153727341101</v>
       </c>
     </row>
@@ -1308,7 +1308,7 @@
       <c r="N23" s="8">
         <v>0.81012520400250099</v>
       </c>
-      <c r="O23" s="16">
+      <c r="O23" s="14">
         <v>1.54015337377857</v>
       </c>
     </row>
@@ -1348,7 +1348,7 @@
       <c r="N24" s="8">
         <v>0.49549295194309001</v>
       </c>
-      <c r="O24" s="16">
+      <c r="O24" s="14">
         <v>1.2534627629772299</v>
       </c>
     </row>
@@ -1388,47 +1388,47 @@
       <c r="N25" s="8">
         <v>-0.23108943334481899</v>
       </c>
-      <c r="O25" s="16">
+      <c r="O25" s="14">
         <v>1.03983102283011</v>
       </c>
     </row>
     <row r="26" spans="2:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="18">
+      <c r="B26" s="16">
         <v>90</v>
       </c>
-      <c r="C26" s="19">
+      <c r="C26" s="17">
         <v>1.2</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="18">
         <v>21.978349979940901</v>
       </c>
-      <c r="E26" s="20">
+      <c r="E26" s="18">
         <v>21.900503608453501</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="18">
         <v>-0.35419570421925001</v>
       </c>
-      <c r="G26" s="20">
+      <c r="G26" s="18">
         <v>0.76803209562278596</v>
       </c>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20">
+      <c r="H26" s="18"/>
+      <c r="I26" s="18">
         <v>21.9179756078256</v>
       </c>
-      <c r="J26" s="20">
+      <c r="J26" s="18">
         <v>-0.27469929348960498</v>
       </c>
-      <c r="K26" s="20">
+      <c r="K26" s="18">
         <v>0.76989210076095704</v>
       </c>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20">
+      <c r="L26" s="18"/>
+      <c r="M26" s="18">
         <v>21.9456381125913</v>
       </c>
-      <c r="N26" s="20">
+      <c r="N26" s="18">
         <v>-0.148836775186896</v>
       </c>
-      <c r="O26" s="21">
+      <c r="O26" s="19">
         <v>0.77705283351769705</v>
       </c>
     </row>
@@ -1468,7 +1468,7 @@
       <c r="N27" s="8">
         <v>0.83317706657309298</v>
       </c>
-      <c r="O27" s="16">
+      <c r="O27" s="14">
         <v>3.4264023113648499</v>
       </c>
     </row>
@@ -1508,7 +1508,7 @@
       <c r="N28" s="8">
         <v>1.34172630015488</v>
       </c>
-      <c r="O28" s="16">
+      <c r="O28" s="14">
         <v>2.20804822397429</v>
       </c>
     </row>
@@ -1548,7 +1548,7 @@
       <c r="N29" s="8">
         <v>0.76376048174275801</v>
       </c>
-      <c r="O29" s="16">
+      <c r="O29" s="14">
         <v>1.82929251896423</v>
       </c>
     </row>
@@ -1588,7 +1588,7 @@
       <c r="N30" s="8">
         <v>8.6083819840957296E-2</v>
       </c>
-      <c r="O30" s="16">
+      <c r="O30" s="14">
         <v>1.5524757545008601</v>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       <c r="N31" s="8">
         <v>6.6673990373937297E-3</v>
       </c>
-      <c r="O31" s="16">
+      <c r="O31" s="14">
         <v>1.34810241396047</v>
       </c>
     </row>
@@ -1668,7 +1668,7 @@
       <c r="N32" s="8">
         <v>-0.16943307847886899</v>
       </c>
-      <c r="O32" s="16">
+      <c r="O32" s="14">
         <v>1.1820341637386</v>
       </c>
     </row>
@@ -1708,7 +1708,7 @@
       <c r="N33" s="9">
         <v>0.51414225042692596</v>
       </c>
-      <c r="O33" s="17">
+      <c r="O33" s="15">
         <v>0.952016386836538</v>
       </c>
     </row>
@@ -1719,23 +1719,23 @@
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="12">
+      <c r="E36" s="25">
         <v>0.8</v>
       </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="12">
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="25">
         <v>1</v>
       </c>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="12">
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="25">
         <v>1.2</v>
       </c>
-      <c r="N36" s="12"/>
-      <c r="O36" s="14"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="26"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B37" s="5"/>
@@ -1767,7 +1767,7 @@
       <c r="N37" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O37" s="15" t="s">
+      <c r="O37" s="13" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1791,45 +1791,45 @@
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
-      <c r="O38" s="15"/>
+      <c r="O38" s="13"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B39" s="22">
+      <c r="B39" s="20">
         <v>30</v>
       </c>
-      <c r="C39" s="23">
+      <c r="C39" s="21">
         <v>0.8</v>
       </c>
-      <c r="D39" s="24">
+      <c r="D39" s="22">
         <v>6.5836656820333897E-3</v>
       </c>
-      <c r="E39" s="24">
+      <c r="E39" s="22">
         <v>6.0990083404018902E-3</v>
       </c>
-      <c r="F39" s="24">
+      <c r="F39" s="22">
         <v>-7.3615120365864497</v>
       </c>
-      <c r="G39" s="24">
+      <c r="G39" s="22">
         <v>13.400164774357499</v>
       </c>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24">
+      <c r="H39" s="22"/>
+      <c r="I39" s="22">
         <v>7.1357057405206804E-3</v>
       </c>
-      <c r="J39" s="24">
+      <c r="J39" s="22">
         <v>8.3849953073071894</v>
       </c>
-      <c r="K39" s="24">
+      <c r="K39" s="22">
         <v>14.4734351967858</v>
       </c>
-      <c r="L39" s="24"/>
-      <c r="M39" s="24">
+      <c r="L39" s="22"/>
+      <c r="M39" s="22">
         <v>7.6664009913129001E-3</v>
       </c>
-      <c r="N39" s="24">
+      <c r="N39" s="22">
         <v>16.445782054733701</v>
       </c>
-      <c r="O39" s="25">
+      <c r="O39" s="23">
         <v>15.020548115025401</v>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       <c r="N40" s="8">
         <v>-0.25498101948077201</v>
       </c>
-      <c r="O40" s="16">
+      <c r="O40" s="14">
         <v>2.7999889262697799</v>
       </c>
     </row>
@@ -1909,7 +1909,7 @@
       <c r="N41" s="8">
         <v>4.9877949300578601E-2</v>
       </c>
-      <c r="O41" s="16">
+      <c r="O41" s="14">
         <v>1.61204013152546</v>
       </c>
     </row>
@@ -1949,7 +1949,7 @@
       <c r="N42" s="8">
         <v>-0.16898131394801899</v>
       </c>
-      <c r="O42" s="16">
+      <c r="O42" s="14">
         <v>1.00028756999917</v>
       </c>
     </row>
@@ -1989,7 +1989,7 @@
       <c r="N43" s="8">
         <v>0.19092980357808001</v>
       </c>
-      <c r="O43" s="16">
+      <c r="O43" s="14">
         <v>0.63692484548388195</v>
       </c>
     </row>
@@ -2029,7 +2029,7 @@
       <c r="N44" s="8">
         <v>-0.403004482428307</v>
       </c>
-      <c r="O44" s="16">
+      <c r="O44" s="14">
         <v>0.40806764194017098</v>
       </c>
     </row>
@@ -2069,47 +2069,47 @@
       <c r="N45" s="8">
         <v>-0.19208306973869299</v>
       </c>
-      <c r="O45" s="16">
+      <c r="O45" s="14">
         <v>0.166270730575001</v>
       </c>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B46" s="22">
+      <c r="B46" s="20">
         <v>90</v>
       </c>
-      <c r="C46" s="23">
+      <c r="C46" s="21">
         <v>0.8</v>
       </c>
-      <c r="D46" s="24">
+      <c r="D46" s="22">
         <v>9.2322034903307995E-2</v>
       </c>
-      <c r="E46" s="24">
+      <c r="E46" s="22">
         <v>9.1254642158093702E-2</v>
       </c>
-      <c r="F46" s="24">
+      <c r="F46" s="22">
         <v>-1.15616249829456</v>
       </c>
-      <c r="G46" s="24">
+      <c r="G46" s="22">
         <v>3.63535493692022</v>
       </c>
-      <c r="H46" s="24"/>
-      <c r="I46" s="24">
+      <c r="H46" s="22"/>
+      <c r="I46" s="22">
         <v>8.9028382015022806E-2</v>
       </c>
-      <c r="J46" s="24">
+      <c r="J46" s="22">
         <v>-3.5675696400480401</v>
       </c>
-      <c r="K46" s="24">
+      <c r="K46" s="22">
         <v>3.5991181493735298</v>
       </c>
-      <c r="L46" s="24"/>
-      <c r="M46" s="24">
+      <c r="L46" s="22"/>
+      <c r="M46" s="22">
         <v>9.0961160072044897E-2</v>
       </c>
-      <c r="N46" s="24">
+      <c r="N46" s="22">
         <v>-1.47405203176931</v>
       </c>
-      <c r="O46" s="25">
+      <c r="O46" s="23">
         <v>3.6361294274278801</v>
       </c>
     </row>
@@ -2149,7 +2149,7 @@
       <c r="N47" s="8">
         <v>1.53892279917619</v>
       </c>
-      <c r="O47" s="16">
+      <c r="O47" s="14">
         <v>1.7786045379995301</v>
       </c>
     </row>
@@ -2189,7 +2189,7 @@
       <c r="N48" s="8">
         <v>-0.293624840076744</v>
       </c>
-      <c r="O48" s="16">
+      <c r="O48" s="14">
         <v>1.3145474410993101</v>
       </c>
     </row>
@@ -2229,7 +2229,7 @@
       <c r="N49" s="8">
         <v>0.27647145271405299</v>
       </c>
-      <c r="O49" s="16">
+      <c r="O49" s="14">
         <v>1.0047016276659999</v>
       </c>
     </row>
@@ -2269,7 +2269,7 @@
       <c r="N50" s="8">
         <v>-5.3382880391829098E-2</v>
       </c>
-      <c r="O50" s="16">
+      <c r="O50" s="14">
         <v>0.77929250523308702</v>
       </c>
     </row>
@@ -2309,47 +2309,47 @@
       <c r="N51" s="8">
         <v>-0.34083788968218698</v>
       </c>
-      <c r="O51" s="16">
+      <c r="O51" s="14">
         <v>0.61067813911291602</v>
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B52" s="18">
+      <c r="B52" s="16">
         <v>90</v>
       </c>
-      <c r="C52" s="19">
+      <c r="C52" s="17">
         <v>1.2</v>
       </c>
-      <c r="D52" s="20">
+      <c r="D52" s="18">
         <v>0.914578087307654</v>
       </c>
-      <c r="E52" s="20">
+      <c r="E52" s="18">
         <v>0.91421065318796801</v>
       </c>
-      <c r="F52" s="20">
+      <c r="F52" s="18">
         <v>-4.0175259476761198E-2</v>
       </c>
-      <c r="G52" s="20">
+      <c r="G52" s="18">
         <v>0.37883530037201102</v>
       </c>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20">
+      <c r="H52" s="18"/>
+      <c r="I52" s="18">
         <v>0.91366483033818302</v>
       </c>
-      <c r="J52" s="20">
+      <c r="J52" s="18">
         <v>-9.9855548928645704E-2</v>
       </c>
-      <c r="K52" s="20">
+      <c r="K52" s="18">
         <v>0.38012286320108302</v>
       </c>
-      <c r="L52" s="20"/>
-      <c r="M52" s="20">
+      <c r="L52" s="18"/>
+      <c r="M52" s="18">
         <v>0.91185400757500201</v>
       </c>
-      <c r="N52" s="20">
+      <c r="N52" s="18">
         <v>-0.29785097308300701</v>
       </c>
-      <c r="O52" s="21">
+      <c r="O52" s="19">
         <v>0.38397302923898102</v>
       </c>
     </row>
@@ -2389,7 +2389,7 @@
       <c r="N53" s="8">
         <v>-0.95281923616938702</v>
       </c>
-      <c r="O53" s="16">
+      <c r="O53" s="14">
         <v>2.3953967571798098</v>
       </c>
     </row>
@@ -2429,7 +2429,7 @@
       <c r="N54" s="8">
         <v>0.47858669372380802</v>
       </c>
-      <c r="O54" s="16">
+      <c r="O54" s="14">
         <v>1.4987725112797601</v>
       </c>
     </row>
@@ -2469,7 +2469,7 @@
       <c r="N55" s="8">
         <v>0.37332374653268502</v>
       </c>
-      <c r="O55" s="16">
+      <c r="O55" s="14">
         <v>1.22192309041227</v>
       </c>
     </row>
@@ -2509,7 +2509,7 @@
       <c r="N56" s="8">
         <v>-0.22602004876753401</v>
       </c>
-      <c r="O56" s="16">
+      <c r="O56" s="14">
         <v>1.01201130526215</v>
       </c>
     </row>
@@ -2549,7 +2549,7 @@
       <c r="N57" s="8">
         <v>-0.22556527383279801</v>
       </c>
-      <c r="O57" s="16">
+      <c r="O57" s="14">
         <v>0.84897720300260004</v>
       </c>
     </row>
@@ -2589,7 +2589,7 @@
       <c r="N58" s="8">
         <v>-9.8190745492271095E-2</v>
       </c>
-      <c r="O58" s="16">
+      <c r="O58" s="14">
         <v>0.71756259293927105</v>
       </c>
     </row>
@@ -2629,7 +2629,7 @@
       <c r="N59" s="9">
         <v>0.19330185160193999</v>
       </c>
-      <c r="O59" s="17">
+      <c r="O59" s="15">
         <v>0.52566204754472601</v>
       </c>
     </row>
@@ -2651,7 +2651,7 @@
   <dimension ref="B1:O59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2659,24 +2659,29 @@
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="1" customWidth="1"/>
-    <col min="5" max="7" width="15.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="3.5" style="1" customWidth="1"/>
-    <col min="9" max="11" width="15.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="3.5" style="1" customWidth="1"/>
-    <col min="13" max="15" width="15.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="5" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.2">
@@ -2737,7 +2742,7 @@
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="24">
         <v>43171</v>
       </c>
     </row>
@@ -2745,7 +2750,7 @@
       <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="24">
         <v>44175</v>
       </c>
     </row>
@@ -2756,23 +2761,23 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="12">
+      <c r="E10" s="25">
         <v>0.8</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="12">
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="25">
         <v>1</v>
       </c>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="12">
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="25">
         <v>1.2</v>
       </c>
-      <c r="N10" s="12"/>
-      <c r="O10" s="14"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="26"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
@@ -2804,7 +2809,7 @@
       <c r="N11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="O11" s="15" t="s">
+      <c r="O11" s="13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2828,45 +2833,45 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
-      <c r="O12" s="15"/>
+      <c r="O12" s="13"/>
     </row>
     <row r="13" spans="2:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="22">
+      <c r="B13" s="20">
         <v>30</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="21">
         <v>0.8</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="22">
         <v>8.7503327040480305E-2</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="22">
         <v>9.0320216905852901E-2</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="22">
         <v>3.2191802993609202</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="22">
         <v>10.291832320856599</v>
       </c>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24">
+      <c r="H13" s="22"/>
+      <c r="I13" s="22">
         <v>0.103294776273416</v>
       </c>
-      <c r="J13" s="24">
+      <c r="J13" s="22">
         <v>18.0466843570767</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K13" s="22">
         <v>11.3829349490002</v>
       </c>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24">
+      <c r="L13" s="22"/>
+      <c r="M13" s="22">
         <v>0.12384777281505099</v>
       </c>
-      <c r="N13" s="24">
+      <c r="N13" s="22">
         <v>41.5349301607217</v>
       </c>
-      <c r="O13" s="25">
+      <c r="O13" s="23">
         <v>12.6383994511389</v>
       </c>
     </row>
@@ -2906,7 +2911,7 @@
       <c r="N14" s="8">
         <v>9.4828988904140594</v>
       </c>
-      <c r="O14" s="16">
+      <c r="O14" s="14">
         <v>3.4744051521374399</v>
       </c>
     </row>
@@ -2946,7 +2951,7 @@
       <c r="N15" s="8">
         <v>2.8788333389047298</v>
       </c>
-      <c r="O15" s="16">
+      <c r="O15" s="14">
         <v>2.2251368714053901</v>
       </c>
     </row>
@@ -2986,7 +2991,7 @@
       <c r="N16" s="8">
         <v>2.8086022790924701</v>
       </c>
-      <c r="O16" s="16">
+      <c r="O16" s="14">
         <v>1.59828599885997</v>
       </c>
     </row>
@@ -3026,7 +3031,7 @@
       <c r="N17" s="8">
         <v>0.26584331502890102</v>
       </c>
-      <c r="O17" s="16">
+      <c r="O17" s="14">
         <v>1.1843513207154299</v>
       </c>
     </row>
@@ -3066,7 +3071,7 @@
       <c r="N18" s="8">
         <v>0.47432605624295898</v>
       </c>
-      <c r="O18" s="16">
+      <c r="O18" s="14">
         <v>0.93718871782310997</v>
       </c>
     </row>
@@ -3106,47 +3111,47 @@
       <c r="N19" s="8">
         <v>0.69189383515696201</v>
       </c>
-      <c r="O19" s="16">
+      <c r="O19" s="14">
         <v>0.64016437011840699</v>
       </c>
     </row>
     <row r="20" spans="2:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="22">
+      <c r="B20" s="20">
         <v>90</v>
       </c>
-      <c r="C20" s="23">
+      <c r="C20" s="21">
         <v>0.8</v>
       </c>
-      <c r="D20" s="24">
+      <c r="D20" s="22">
         <v>1.15910993284727</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="22">
         <v>1.1659188156218301</v>
       </c>
-      <c r="F20" s="24">
+      <c r="F20" s="22">
         <v>0.58742338251168902</v>
       </c>
-      <c r="G20" s="24">
+      <c r="G20" s="22">
         <v>3.9491861576849399</v>
       </c>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24">
+      <c r="H20" s="22"/>
+      <c r="I20" s="22">
         <v>1.16087412591106</v>
       </c>
-      <c r="J20" s="24">
+      <c r="J20" s="22">
         <v>0.152202393732565</v>
       </c>
-      <c r="K20" s="24">
+      <c r="K20" s="22">
         <v>3.97733450959735</v>
       </c>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24">
+      <c r="L20" s="22"/>
+      <c r="M20" s="22">
         <v>1.20789222127615</v>
       </c>
-      <c r="N20" s="24">
+      <c r="N20" s="22">
         <v>4.2085989470429102</v>
       </c>
-      <c r="O20" s="25">
+      <c r="O20" s="23">
         <v>4.0892448963528798</v>
       </c>
     </row>
@@ -3186,7 +3191,7 @@
       <c r="N21" s="8">
         <v>1.14270528066886</v>
       </c>
-      <c r="O21" s="16">
+      <c r="O21" s="14">
         <v>2.3564963116199298</v>
       </c>
     </row>
@@ -3226,7 +3231,7 @@
       <c r="N22" s="8">
         <v>-0.62403426269921602</v>
       </c>
-      <c r="O22" s="16">
+      <c r="O22" s="14">
         <v>1.8911142266307299</v>
       </c>
     </row>
@@ -3266,7 +3271,7 @@
       <c r="N23" s="8">
         <v>-1.35726482815014</v>
       </c>
-      <c r="O23" s="16">
+      <c r="O23" s="14">
         <v>1.5793561812075001</v>
       </c>
     </row>
@@ -3306,7 +3311,7 @@
       <c r="N24" s="8">
         <v>0.25481003670964503</v>
       </c>
-      <c r="O24" s="16">
+      <c r="O24" s="14">
         <v>1.35319501783562</v>
       </c>
     </row>
@@ -3346,47 +3351,47 @@
       <c r="N25" s="8">
         <v>0.460516813318887</v>
       </c>
-      <c r="O25" s="16">
+      <c r="O25" s="14">
         <v>1.1722932117503</v>
       </c>
     </row>
     <row r="26" spans="2:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="18">
+      <c r="B26" s="16">
         <v>90</v>
       </c>
-      <c r="C26" s="19">
+      <c r="C26" s="17">
         <v>1.2</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="18">
         <v>22.898973558730699</v>
       </c>
-      <c r="E26" s="20">
+      <c r="E26" s="18">
         <v>22.994178573564099</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="18">
         <v>0.41576105841159</v>
       </c>
-      <c r="G26" s="20">
+      <c r="G26" s="18">
         <v>0.909371412255497</v>
       </c>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20">
+      <c r="H26" s="18"/>
+      <c r="I26" s="18">
         <v>22.9225590928625</v>
       </c>
-      <c r="J26" s="20">
+      <c r="J26" s="18">
         <v>0.102998215493048</v>
       </c>
-      <c r="K26" s="20">
+      <c r="K26" s="18">
         <v>0.90922330174847099</v>
       </c>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20">
+      <c r="L26" s="18"/>
+      <c r="M26" s="18">
         <v>23.049749744070802</v>
       </c>
-      <c r="N26" s="20">
+      <c r="N26" s="18">
         <v>0.65844080283122297</v>
       </c>
-      <c r="O26" s="21">
+      <c r="O26" s="19">
         <v>0.91753481034992901</v>
       </c>
     </row>
@@ -3426,7 +3431,7 @@
       <c r="N27" s="8">
         <v>2.1448999525213699</v>
       </c>
-      <c r="O27" s="16">
+      <c r="O27" s="14">
         <v>3.0108968878281601</v>
       </c>
     </row>
@@ -3466,7 +3471,7 @@
       <c r="N28" s="8">
         <v>0.93546767668209896</v>
       </c>
-      <c r="O28" s="16">
+      <c r="O28" s="14">
         <v>2.1427740033647802</v>
       </c>
     </row>
@@ -3506,7 +3511,7 @@
       <c r="N29" s="8">
         <v>1.0108739206476101</v>
       </c>
-      <c r="O29" s="16">
+      <c r="O29" s="14">
         <v>1.8589654125580399</v>
       </c>
     </row>
@@ -3546,7 +3551,7 @@
       <c r="N30" s="8">
         <v>0.87208370090290799</v>
       </c>
-      <c r="O30" s="16">
+      <c r="O30" s="14">
         <v>1.65566749118751</v>
       </c>
     </row>
@@ -3586,7 +3591,7 @@
       <c r="N31" s="8">
         <v>-0.91416251296926998</v>
       </c>
-      <c r="O31" s="16">
+      <c r="O31" s="14">
         <v>1.46504779186558</v>
       </c>
     </row>
@@ -3626,7 +3631,7 @@
       <c r="N32" s="8">
         <v>0.19136386505667699</v>
       </c>
-      <c r="O32" s="16">
+      <c r="O32" s="14">
         <v>1.3144553701917201</v>
       </c>
     </row>
@@ -3666,7 +3671,7 @@
       <c r="N33" s="9">
         <v>0.68715424572025396</v>
       </c>
-      <c r="O33" s="17">
+      <c r="O33" s="15">
         <v>1.10527250410861</v>
       </c>
     </row>
@@ -3677,23 +3682,23 @@
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="12">
+      <c r="E36" s="25">
         <v>0.8</v>
       </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="12">
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="25">
         <v>1</v>
       </c>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="12">
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="25">
         <v>1.2</v>
       </c>
-      <c r="N36" s="12"/>
-      <c r="O36" s="14"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="26"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B37" s="5"/>
@@ -3725,7 +3730,7 @@
       <c r="N37" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O37" s="15" t="s">
+      <c r="O37" s="13" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3749,45 +3754,45 @@
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
-      <c r="O38" s="15"/>
+      <c r="O38" s="13"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B39" s="22">
+      <c r="B39" s="20">
         <v>30</v>
       </c>
-      <c r="C39" s="23">
+      <c r="C39" s="21">
         <v>0.8</v>
       </c>
-      <c r="D39" s="24">
+      <c r="D39" s="22">
         <v>2.6943063272294399E-2</v>
       </c>
-      <c r="E39" s="24">
+      <c r="E39" s="22">
         <v>2.5752601623393101E-2</v>
       </c>
-      <c r="F39" s="24">
+      <c r="F39" s="22">
         <v>-4.4184346704388302</v>
       </c>
-      <c r="G39" s="24">
+      <c r="G39" s="22">
         <v>6.7350728101034596</v>
       </c>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24">
+      <c r="H39" s="22"/>
+      <c r="I39" s="22">
         <v>2.74833242944162E-2</v>
       </c>
-      <c r="J39" s="24">
+      <c r="J39" s="22">
         <v>2.0051952395382799</v>
       </c>
-      <c r="K39" s="24">
+      <c r="K39" s="22">
         <v>6.9656217235903597</v>
       </c>
-      <c r="L39" s="24"/>
-      <c r="M39" s="24">
+      <c r="L39" s="22"/>
+      <c r="M39" s="22">
         <v>3.3142987978607499E-2</v>
       </c>
-      <c r="N39" s="24">
+      <c r="N39" s="22">
         <v>23.011209392394701</v>
       </c>
-      <c r="O39" s="25">
+      <c r="O39" s="23">
         <v>7.6317812190745498</v>
       </c>
     </row>
@@ -3827,7 +3832,7 @@
       <c r="N40" s="8">
         <v>2.4887984482415799</v>
       </c>
-      <c r="O40" s="16">
+      <c r="O40" s="14">
         <v>2.2775653217300502</v>
       </c>
     </row>
@@ -3867,7 +3872,7 @@
       <c r="N41" s="8">
         <v>-9.3209173397336906E-2</v>
       </c>
-      <c r="O41" s="16">
+      <c r="O41" s="14">
         <v>1.4819413015391401</v>
       </c>
     </row>
@@ -3907,7 +3912,7 @@
       <c r="N42" s="8">
         <v>0.368819180545575</v>
       </c>
-      <c r="O42" s="16">
+      <c r="O42" s="14">
         <v>1.02212268089266</v>
       </c>
     </row>
@@ -3947,7 +3952,7 @@
       <c r="N43" s="8">
         <v>-0.38532792207197902</v>
       </c>
-      <c r="O43" s="16">
+      <c r="O43" s="14">
         <v>0.72007611164749796</v>
       </c>
     </row>
@@ -3987,7 +3992,7 @@
       <c r="N44" s="8">
         <v>-0.21057330723692699</v>
       </c>
-      <c r="O44" s="16">
+      <c r="O44" s="14">
         <v>0.51128911015588097</v>
       </c>
     </row>
@@ -4027,47 +4032,47 @@
       <c r="N45" s="8">
         <v>-0.22391931223303499</v>
       </c>
-      <c r="O45" s="16">
+      <c r="O45" s="14">
         <v>0.263700399174497</v>
       </c>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B46" s="22">
+      <c r="B46" s="20">
         <v>90</v>
       </c>
-      <c r="C46" s="23">
+      <c r="C46" s="21">
         <v>0.8</v>
       </c>
-      <c r="D46" s="24">
+      <c r="D46" s="22">
         <v>0.15714668515692801</v>
       </c>
-      <c r="E46" s="24">
+      <c r="E46" s="22">
         <v>0.154834047943292</v>
       </c>
-      <c r="F46" s="24">
+      <c r="F46" s="22">
         <v>-1.4716423775196601</v>
       </c>
-      <c r="G46" s="24">
+      <c r="G46" s="22">
         <v>2.7641119452804799</v>
       </c>
-      <c r="H46" s="24"/>
-      <c r="I46" s="24">
+      <c r="H46" s="22"/>
+      <c r="I46" s="22">
         <v>0.15311651322963299</v>
       </c>
-      <c r="J46" s="24">
+      <c r="J46" s="22">
         <v>-2.5645923891242401</v>
       </c>
-      <c r="K46" s="24">
+      <c r="K46" s="22">
         <v>2.7521864993945702</v>
       </c>
-      <c r="L46" s="24"/>
-      <c r="M46" s="24">
+      <c r="L46" s="22"/>
+      <c r="M46" s="22">
         <v>0.15928500952399399</v>
       </c>
-      <c r="N46" s="24">
+      <c r="N46" s="22">
         <v>1.3607187227211499</v>
       </c>
-      <c r="O46" s="25">
+      <c r="O46" s="23">
         <v>2.80047627452061</v>
       </c>
     </row>
@@ -4107,7 +4112,7 @@
       <c r="N47" s="8">
         <v>0.43933424474129501</v>
       </c>
-      <c r="O47" s="16">
+      <c r="O47" s="14">
         <v>1.6178044272430201</v>
       </c>
     </row>
@@ -4147,7 +4152,7 @@
       <c r="N48" s="8">
         <v>-6.9072399832448797E-2</v>
       </c>
-      <c r="O48" s="16">
+      <c r="O48" s="14">
         <v>1.2831096851658701</v>
       </c>
     </row>
@@ -4187,7 +4192,7 @@
       <c r="N49" s="8">
         <v>-1.5589677783698701</v>
       </c>
-      <c r="O49" s="16">
+      <c r="O49" s="14">
         <v>1.03982253866075</v>
       </c>
     </row>
@@ -4227,7 +4232,7 @@
       <c r="N50" s="8">
         <v>-0.138752824797514</v>
       </c>
-      <c r="O50" s="16">
+      <c r="O50" s="14">
         <v>0.85467555212685198</v>
       </c>
     </row>
@@ -4267,47 +4272,47 @@
       <c r="N51" s="8">
         <v>3.29242061978492E-2</v>
       </c>
-      <c r="O51" s="16">
+      <c r="O51" s="14">
         <v>0.70825687700804096</v>
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B52" s="18">
+      <c r="B52" s="16">
         <v>90</v>
       </c>
-      <c r="C52" s="19">
+      <c r="C52" s="17">
         <v>1.2</v>
       </c>
-      <c r="D52" s="20">
+      <c r="D52" s="18">
         <v>0.86716314103824299</v>
       </c>
-      <c r="E52" s="20">
+      <c r="E52" s="18">
         <v>0.871648984826083</v>
       </c>
-      <c r="F52" s="20">
+      <c r="F52" s="18">
         <v>0.51730102163568603</v>
       </c>
-      <c r="G52" s="20">
+      <c r="G52" s="18">
         <v>0.492313628198841</v>
       </c>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20">
+      <c r="H52" s="18"/>
+      <c r="I52" s="18">
         <v>0.87032780807834598</v>
       </c>
-      <c r="J52" s="20">
+      <c r="J52" s="18">
         <v>0.36494482875659501</v>
       </c>
-      <c r="K52" s="20">
+      <c r="K52" s="18">
         <v>0.492967595797142</v>
       </c>
-      <c r="L52" s="20"/>
-      <c r="M52" s="20">
+      <c r="L52" s="18"/>
+      <c r="M52" s="18">
         <v>0.86839156451211197</v>
       </c>
-      <c r="N52" s="20">
+      <c r="N52" s="18">
         <v>0.141660019404759</v>
       </c>
-      <c r="O52" s="21">
+      <c r="O52" s="19">
         <v>0.49780523521572601</v>
       </c>
     </row>
@@ -4347,7 +4352,7 @@
       <c r="N53" s="8">
         <v>0.85656363404446401</v>
       </c>
-      <c r="O53" s="16">
+      <c r="O53" s="14">
         <v>2.0821465497131002</v>
       </c>
     </row>
@@ -4387,7 +4392,7 @@
       <c r="N54" s="8">
         <v>0.59852971489134099</v>
       </c>
-      <c r="O54" s="16">
+      <c r="O54" s="14">
         <v>1.4468889232996101</v>
       </c>
     </row>
@@ -4427,7 +4432,7 @@
       <c r="N55" s="8">
         <v>0.38459578354006302</v>
       </c>
-      <c r="O55" s="16">
+      <c r="O55" s="14">
         <v>1.2359733440624501</v>
       </c>
     </row>
@@ -4467,7 +4472,7 @@
       <c r="N56" s="8">
         <v>0.38551117329190998</v>
       </c>
-      <c r="O56" s="16">
+      <c r="O56" s="14">
         <v>1.0691803251806899</v>
       </c>
     </row>
@@ -4507,7 +4512,7 @@
       <c r="N57" s="8">
         <v>-0.69027421835701297</v>
       </c>
-      <c r="O57" s="16">
+      <c r="O57" s="14">
         <v>0.93180143304126095</v>
       </c>
     </row>
@@ -4547,7 +4552,7 @@
       <c r="N58" s="8">
         <v>0.310822431379978</v>
       </c>
-      <c r="O58" s="16">
+      <c r="O58" s="14">
         <v>0.81829096538488899</v>
       </c>
     </row>
@@ -4587,7 +4592,7 @@
       <c r="N59" s="9">
         <v>0.56432796124190798</v>
       </c>
-      <c r="O59" s="17">
+      <c r="O59" s="15">
         <v>0.64664161042457502</v>
       </c>
     </row>

</xml_diff>